<commit_message>
RDM-2055 Add new column in spreadsheet.
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V30_RDM-2054.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V30_RDM-2054.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-5360" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="-5360" yWindow="460" windowWidth="38400" windowHeight="16560" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -15990,7 +15990,7 @@
   <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="N1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -16244,7 +16244,7 @@
         <v>176</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>

</xml_diff>

<commit_message>
RDM-2055 Make sure we allow empty values in spreadsheet to make it consistent with show_summary column.
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V30_RDM-2054.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V30_RDM-2054.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-5360" yWindow="460" windowWidth="38400" windowHeight="16560" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="-5640" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="277">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -15989,8 +15989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="N1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="M1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -16288,9 +16288,7 @@
       <c r="Q6" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="R6" s="4" t="s">
-        <v>172</v>
-      </c>
+      <c r="R6" s="4"/>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>

</xml_diff>